<commit_message>
update: indexing complete, gitbook okay, errors might exist for pdf
</commit_message>
<xml_diff>
--- a/_index/index.xlsx
+++ b/_index/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pilha\pipetbooks\basic\_index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1F1DD-33DD-4F73-B13E-31D55E726294}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77CD5CF-3C79-4561-8589-210CAAB256A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECD2918D-62A0-4856-BE13-E9328C629C28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="418">
   <si>
     <t>대각행렬</t>
   </si>
@@ -907,6 +907,399 @@
   </si>
   <si>
     <t>\$COVARIANCE (\$COV, \$COVAR)</t>
+  </si>
+  <si>
+    <t>\$DATA</t>
+  </si>
+  <si>
+    <t>\$DES</t>
+  </si>
+  <si>
+    <t>\$ERROR</t>
+  </si>
+  <si>
+    <t>\$ESTIMATION\|\$EST</t>
+  </si>
+  <si>
+    <t>\$ESTIMATION (\$EST)</t>
+  </si>
+  <si>
+    <t>\$INPUT</t>
+  </si>
+  <si>
+    <t>\$MODEL</t>
+  </si>
+  <si>
+    <t>\$MSFI</t>
+  </si>
+  <si>
+    <t>\$OMEGA</t>
+  </si>
+  <si>
+    <t>\$OMEGA BLOCK</t>
+  </si>
+  <si>
+    <t>\$OMEGA BIAGONAL</t>
+  </si>
+  <si>
+    <t>\$PK</t>
+  </si>
+  <si>
+    <t>\$PRED</t>
+  </si>
+  <si>
+    <t>\$PROBLEM</t>
+  </si>
+  <si>
+    <t>\$SCATTERPLOT\|\$SCAT</t>
+  </si>
+  <si>
+    <t>\$SIGMA</t>
+  </si>
+  <si>
+    <t>\$SIGMA DIAGONAL</t>
+  </si>
+  <si>
+    <t>\$SIMULATION\|\$SIM</t>
+  </si>
+  <si>
+    <t>\$SCATTERPLOT (\$SCAT)</t>
+  </si>
+  <si>
+    <t>\$SIMULATION (\$SIM)</t>
+  </si>
+  <si>
+    <t>\$SIMULATION ONLYSIM</t>
+  </si>
+  <si>
+    <t>\$SUBROUTINE</t>
+  </si>
+  <si>
+    <t>\$TABLE</t>
+  </si>
+  <si>
+    <t>\$THETA</t>
+  </si>
+  <si>
+    <t>\$TOL</t>
+  </si>
+  <si>
+    <t>ACCEPT</t>
+  </si>
+  <si>
+    <t>ADDL</t>
+  </si>
+  <si>
+    <t>ADVAN1</t>
+  </si>
+  <si>
+    <t>ADVAN2</t>
+  </si>
+  <si>
+    <t>ADVAN3</t>
+  </si>
+  <si>
+    <t>ADVAN4</t>
+  </si>
+  <si>
+    <t>ADVAN5</t>
+  </si>
+  <si>
+    <t>ADVAN6</t>
+  </si>
+  <si>
+    <t>ADVAN7</t>
+  </si>
+  <si>
+    <t>ADVAN8</t>
+  </si>
+  <si>
+    <t>ADVAN9</t>
+  </si>
+  <si>
+    <t>ADVAN10</t>
+  </si>
+  <si>
+    <t>ADVAN11</t>
+  </si>
+  <si>
+    <t>ADVAN12</t>
+  </si>
+  <si>
+    <t>ADVAN13</t>
+  </si>
+  <si>
+    <t>ALAG</t>
+  </si>
+  <si>
+    <t>AMT</t>
+  </si>
+  <si>
+    <t>BAYES</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>CALLFL = 0</t>
+  </si>
+  <si>
+    <t>CHECKOUT</t>
+  </si>
+  <si>
+    <t>CMT</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>COMPRESS</t>
+  </si>
+  <si>
+    <t>CONT</t>
+  </si>
+  <si>
+    <t>CPRED</t>
+  </si>
+  <si>
+    <t>CPREDI</t>
+  </si>
+  <si>
+    <t>CRES</t>
+  </si>
+  <si>
+    <t>CRESI</t>
+  </si>
+  <si>
+    <t>CWRES</t>
+  </si>
+  <si>
+    <t>CWRESI</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>DADT(i)</t>
+  </si>
+  <si>
+    <t>DAT1</t>
+  </si>
+  <si>
+    <t>DAT2</t>
+  </si>
+  <si>
+    <t>DAT3</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>DATE=DROP</t>
+  </si>
+  <si>
+    <t>DEFDOS</t>
+  </si>
+  <si>
+    <t>DEFOBS</t>
+  </si>
+  <si>
+    <t>DROP</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>ETABAR</t>
+  </si>
+  <si>
+    <t>EVID</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>FDATA</t>
+  </si>
+  <si>
+    <t>F_FLAG</t>
+  </si>
+  <si>
+    <t>FILE=</t>
+  </si>
+  <si>
+    <t>FIRSTONLY</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IF-THEN</t>
+  </si>
+  <si>
+    <t>IGNORE</t>
+  </si>
+  <si>
+    <t>INTERACTION</t>
+  </si>
+  <si>
+    <t>IPRED</t>
+  </si>
+  <si>
+    <t>IREP</t>
+  </si>
+  <si>
+    <t>IRES</t>
+  </si>
+  <si>
+    <t>IWRES</t>
+  </si>
+  <si>
+    <t>LAPLACIAN</t>
+  </si>
+  <si>
+    <t>LFORMAT</t>
+  </si>
+  <si>
+    <t>LIKELIHOOD</t>
+  </si>
+  <si>
+    <t>MATRIX = R</t>
+  </si>
+  <si>
+    <t>MATRIX = S</t>
+  </si>
+  <si>
+    <t>MAXEVAL</t>
+  </si>
+  <si>
+    <t>MAXEVAL=0</t>
+  </si>
+  <si>
+    <t>MDV</t>
+  </si>
+  <si>
+    <t>MPAST</t>
+  </si>
+  <si>
+    <t>MSF</t>
+  </si>
+  <si>
+    <t>MSFO</t>
+  </si>
+  <si>
+    <t>MTIME</t>
+  </si>
+  <si>
+    <t>NOABORT</t>
+  </si>
+  <si>
+    <t>NOAPPEND</t>
+  </si>
+  <si>
+    <t>NOHEADER</t>
+  </si>
+  <si>
+    <t>NOOMEGABOUNTTEST</t>
+  </si>
+  <si>
+    <t>NOPRINT</t>
+  </si>
+  <si>
+    <t>NOSIGMABOUNDTEST</t>
+  </si>
+  <si>
+    <t>NOTHETABOUNDTEST</t>
+  </si>
+  <si>
+    <t>NSIG</t>
+  </si>
+  <si>
+    <t>NSUB</t>
+  </si>
+  <si>
+    <t>OBSERVATIONS ONLY</t>
+  </si>
+  <si>
+    <t>ONEHEADER</t>
+  </si>
+  <si>
+    <t>ONLYSIM</t>
+  </si>
+  <si>
+    <t>PCMT</t>
+  </si>
+  <si>
+    <t>POSTHOC</t>
+  </si>
+  <si>
+    <t>PRED</t>
+  </si>
+  <si>
+    <t>PREDPP</t>
+  </si>
+  <si>
+    <t>PRINT=E</t>
+  </si>
+  <si>
+    <t>PRINT=n</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>RFORMAT</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SIGDIGITS\|SIGDIG</t>
+  </si>
+  <si>
+    <t>SORT</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>SUBPROBLEMS</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>TOL</t>
+  </si>
+  <si>
+    <t>TRANS</t>
+  </si>
+  <si>
+    <t>TRANS2</t>
+  </si>
+  <si>
+    <t>TRUE=FINAL</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>WRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y\ </t>
   </si>
 </sst>
 </file>
@@ -1266,11 +1659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B1A01-E184-4A00-A964-5F70651C46A8}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3699,7 +4092,7 @@
     </row>
     <row r="102" spans="2:7">
       <c r="E102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F102" t="s">
         <v>285</v>
@@ -3710,7 +4103,7 @@
     </row>
     <row r="103" spans="2:7">
       <c r="E103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" t="s">
         <v>284</v>
@@ -3721,13 +4114,1454 @@
     </row>
     <row r="104" spans="2:7">
       <c r="E104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" t="s">
         <v>286</v>
       </c>
       <c r="G104" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105" t="s">
+        <v>287</v>
+      </c>
+      <c r="G105" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106" t="s">
+        <v>288</v>
+      </c>
+      <c r="G106" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7">
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107" t="s">
+        <v>289</v>
+      </c>
+      <c r="G107" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7">
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108" t="s">
+        <v>291</v>
+      </c>
+      <c r="G108" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7">
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109" t="s">
+        <v>292</v>
+      </c>
+      <c r="G109" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110" t="s">
+        <v>293</v>
+      </c>
+      <c r="G110" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7">
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111" t="s">
+        <v>294</v>
+      </c>
+      <c r="G111" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7">
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112" t="s">
+        <v>295</v>
+      </c>
+      <c r="G112" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="113" spans="5:7">
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113" t="s">
+        <v>296</v>
+      </c>
+      <c r="G113" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="114" spans="5:7">
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114" t="s">
+        <v>297</v>
+      </c>
+      <c r="G114" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="115" spans="5:7">
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115" t="s">
+        <v>298</v>
+      </c>
+      <c r="G115" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="116" spans="5:7">
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116" t="s">
+        <v>299</v>
+      </c>
+      <c r="G116" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="117" spans="5:7">
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117" t="s">
+        <v>300</v>
+      </c>
+      <c r="G117" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="118" spans="5:7">
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118" t="s">
+        <v>305</v>
+      </c>
+      <c r="G118" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="119" spans="5:7">
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119" t="s">
+        <v>302</v>
+      </c>
+      <c r="G119" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="120" spans="5:7">
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>303</v>
+      </c>
+      <c r="G120" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="121" spans="5:7">
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121" t="s">
+        <v>306</v>
+      </c>
+      <c r="G121" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="122" spans="5:7">
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122" t="s">
+        <v>307</v>
+      </c>
+      <c r="G122" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="123" spans="5:7">
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123" t="s">
+        <v>308</v>
+      </c>
+      <c r="G123" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="124" spans="5:7">
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124" t="s">
+        <v>309</v>
+      </c>
+      <c r="G124" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="125" spans="5:7">
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125" t="s">
+        <v>310</v>
+      </c>
+      <c r="G125" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="126" spans="5:7">
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126" t="s">
+        <v>311</v>
+      </c>
+      <c r="G126" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="127" spans="5:7">
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127" t="s">
+        <v>312</v>
+      </c>
+      <c r="G127" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="128" spans="5:7">
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128" t="s">
+        <v>313</v>
+      </c>
+      <c r="G128" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="129" spans="5:7">
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129" t="s">
+        <v>314</v>
+      </c>
+      <c r="G129" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="130" spans="5:7">
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130" t="s">
+        <v>315</v>
+      </c>
+      <c r="G130" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="131" spans="5:7">
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131" t="s">
+        <v>316</v>
+      </c>
+      <c r="G131" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="132" spans="5:7">
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132" t="s">
+        <v>317</v>
+      </c>
+      <c r="G132" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="133" spans="5:7">
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133" t="s">
+        <v>318</v>
+      </c>
+      <c r="G133" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="134" spans="5:7">
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134" t="s">
+        <v>319</v>
+      </c>
+      <c r="G134" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="135" spans="5:7">
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135" t="s">
+        <v>320</v>
+      </c>
+      <c r="G135" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="136" spans="5:7">
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136" t="s">
+        <v>321</v>
+      </c>
+      <c r="G136" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="137" spans="5:7">
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137" t="s">
+        <v>322</v>
+      </c>
+      <c r="G137" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="138" spans="5:7">
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138" t="s">
+        <v>323</v>
+      </c>
+      <c r="G138" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="139" spans="5:7">
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>324</v>
+      </c>
+      <c r="G139" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="140" spans="5:7">
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140" t="s">
+        <v>325</v>
+      </c>
+      <c r="G140" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="141" spans="5:7">
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141" t="s">
+        <v>326</v>
+      </c>
+      <c r="G141" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="142" spans="5:7">
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142" t="s">
+        <v>327</v>
+      </c>
+      <c r="G142" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="143" spans="5:7">
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143" t="s">
+        <v>328</v>
+      </c>
+      <c r="G143" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="144" spans="5:7">
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144" t="s">
+        <v>329</v>
+      </c>
+      <c r="G144" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="145" spans="5:7">
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" t="s">
+        <v>330</v>
+      </c>
+      <c r="G145" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="146" spans="5:7">
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146" t="s">
+        <v>331</v>
+      </c>
+      <c r="G146" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="147" spans="5:7">
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147" t="s">
+        <v>332</v>
+      </c>
+      <c r="G147" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="148" spans="5:7">
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148" t="s">
+        <v>333</v>
+      </c>
+      <c r="G148" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="149" spans="5:7">
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149" t="s">
+        <v>334</v>
+      </c>
+      <c r="G149" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="150" spans="5:7">
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150" t="s">
+        <v>335</v>
+      </c>
+      <c r="G150" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="151" spans="5:7">
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151" t="s">
+        <v>336</v>
+      </c>
+      <c r="G151" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="152" spans="5:7">
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152" t="s">
+        <v>337</v>
+      </c>
+      <c r="G152" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="153" spans="5:7">
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153" t="s">
+        <v>338</v>
+      </c>
+      <c r="G153" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="154" spans="5:7">
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154" t="s">
+        <v>339</v>
+      </c>
+      <c r="G154" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="155" spans="5:7">
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155" t="s">
+        <v>340</v>
+      </c>
+      <c r="G155" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="156" spans="5:7">
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156" t="s">
+        <v>341</v>
+      </c>
+      <c r="G156" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="157" spans="5:7">
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157" t="s">
+        <v>342</v>
+      </c>
+      <c r="G157" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="158" spans="5:7">
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158" t="s">
+        <v>343</v>
+      </c>
+      <c r="G158" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="159" spans="5:7">
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159" t="s">
+        <v>344</v>
+      </c>
+      <c r="G159" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="160" spans="5:7">
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160" t="s">
+        <v>345</v>
+      </c>
+      <c r="G160" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="161" spans="5:7">
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161" t="s">
+        <v>346</v>
+      </c>
+      <c r="G161" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="162" spans="5:7">
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162" t="s">
+        <v>347</v>
+      </c>
+      <c r="G162" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="163" spans="5:7">
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163" t="s">
+        <v>348</v>
+      </c>
+      <c r="G163" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="164" spans="5:7">
+      <c r="E164">
+        <v>0</v>
+      </c>
+      <c r="F164" t="s">
+        <v>349</v>
+      </c>
+      <c r="G164" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="165" spans="5:7">
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="F165" t="s">
+        <v>350</v>
+      </c>
+      <c r="G165" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="166" spans="5:7">
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166" t="s">
+        <v>351</v>
+      </c>
+      <c r="G166" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="167" spans="5:7">
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="F167" t="s">
+        <v>352</v>
+      </c>
+      <c r="G167" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="168" spans="5:7">
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="F168" t="s">
+        <v>353</v>
+      </c>
+      <c r="G168" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="169" spans="5:7">
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="F169" t="s">
+        <v>354</v>
+      </c>
+      <c r="G169" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="170" spans="5:7">
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170" t="s">
+        <v>355</v>
+      </c>
+      <c r="G170" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="171" spans="5:7">
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171" t="s">
+        <v>151</v>
+      </c>
+      <c r="G171" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="172" spans="5:7">
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172" t="s">
+        <v>356</v>
+      </c>
+      <c r="G172" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="173" spans="5:7">
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173" t="s">
+        <v>357</v>
+      </c>
+      <c r="G173" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="174" spans="5:7">
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174" t="s">
+        <v>358</v>
+      </c>
+      <c r="G174" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="175" spans="5:7">
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175" t="s">
+        <v>359</v>
+      </c>
+      <c r="G175" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="176" spans="5:7">
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176" t="s">
+        <v>360</v>
+      </c>
+      <c r="G176" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="177" spans="5:7">
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177" t="s">
+        <v>361</v>
+      </c>
+      <c r="G177" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="178" spans="5:7">
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178" t="s">
+        <v>250</v>
+      </c>
+      <c r="G178" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="179" spans="5:7">
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179" t="s">
+        <v>362</v>
+      </c>
+      <c r="G179" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="180" spans="5:7">
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180" t="s">
+        <v>363</v>
+      </c>
+      <c r="G180" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="181" spans="5:7">
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181" t="s">
+        <v>364</v>
+      </c>
+      <c r="G181" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="182" spans="5:7">
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182" t="s">
+        <v>365</v>
+      </c>
+      <c r="G182" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="183" spans="5:7">
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183" t="s">
+        <v>366</v>
+      </c>
+      <c r="G183" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="184" spans="5:7">
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184" t="s">
+        <v>367</v>
+      </c>
+      <c r="G184" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" spans="5:7">
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185" t="s">
+        <v>368</v>
+      </c>
+      <c r="G185" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="186" spans="5:7">
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186" t="s">
+        <v>369</v>
+      </c>
+      <c r="G186" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="187" spans="5:7">
+      <c r="E187">
+        <v>0</v>
+      </c>
+      <c r="F187" t="s">
+        <v>370</v>
+      </c>
+      <c r="G187" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="188" spans="5:7">
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188" t="s">
+        <v>371</v>
+      </c>
+      <c r="G188" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="189" spans="5:7">
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189" t="s">
+        <v>372</v>
+      </c>
+      <c r="G189" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="190" spans="5:7">
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190" t="s">
+        <v>373</v>
+      </c>
+      <c r="G190" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="191" spans="5:7">
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191" t="s">
+        <v>374</v>
+      </c>
+      <c r="G191" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="192" spans="5:7">
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192" t="s">
+        <v>375</v>
+      </c>
+      <c r="G192" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="193" spans="5:7">
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193" t="s">
+        <v>376</v>
+      </c>
+      <c r="G193" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="194" spans="5:7">
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194" t="s">
+        <v>377</v>
+      </c>
+      <c r="G194" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="195" spans="5:7">
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195" t="s">
+        <v>378</v>
+      </c>
+      <c r="G195" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="196" spans="5:7">
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196" t="s">
+        <v>379</v>
+      </c>
+      <c r="G196" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="197" spans="5:7">
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197" t="s">
+        <v>380</v>
+      </c>
+      <c r="G197" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="198" spans="5:7">
+      <c r="E198">
+        <v>0</v>
+      </c>
+      <c r="F198" t="s">
+        <v>381</v>
+      </c>
+      <c r="G198" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="199" spans="5:7">
+      <c r="E199">
+        <v>0</v>
+      </c>
+      <c r="F199" t="s">
+        <v>382</v>
+      </c>
+      <c r="G199" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="200" spans="5:7">
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200" t="s">
+        <v>268</v>
+      </c>
+      <c r="G200" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="201" spans="5:7">
+      <c r="E201">
+        <v>0</v>
+      </c>
+      <c r="F201" t="s">
+        <v>383</v>
+      </c>
+      <c r="G201" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="202" spans="5:7">
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202" t="s">
+        <v>384</v>
+      </c>
+      <c r="G202" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="203" spans="5:7">
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203" t="s">
+        <v>385</v>
+      </c>
+      <c r="G203" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="204" spans="5:7">
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204" t="s">
+        <v>386</v>
+      </c>
+      <c r="G204" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="205" spans="5:7">
+      <c r="E205">
+        <v>0</v>
+      </c>
+      <c r="F205" t="s">
+        <v>387</v>
+      </c>
+      <c r="G205" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="206" spans="5:7">
+      <c r="E206">
+        <v>0</v>
+      </c>
+      <c r="F206" t="s">
+        <v>388</v>
+      </c>
+      <c r="G206" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="207" spans="5:7">
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207" t="s">
+        <v>389</v>
+      </c>
+      <c r="G207" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="208" spans="5:7">
+      <c r="E208">
+        <v>0</v>
+      </c>
+      <c r="F208" t="s">
+        <v>390</v>
+      </c>
+      <c r="G208" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="209" spans="5:7">
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209" t="s">
+        <v>391</v>
+      </c>
+      <c r="G209" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="210" spans="5:7">
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210" t="s">
+        <v>392</v>
+      </c>
+      <c r="G210" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="211" spans="5:7">
+      <c r="E211">
+        <v>0</v>
+      </c>
+      <c r="F211" t="s">
+        <v>393</v>
+      </c>
+      <c r="G211" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="212" spans="5:7">
+      <c r="E212">
+        <v>0</v>
+      </c>
+      <c r="F212" t="s">
+        <v>394</v>
+      </c>
+      <c r="G212" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="213" spans="5:7">
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213" t="s">
+        <v>395</v>
+      </c>
+      <c r="G213" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="214" spans="5:7">
+      <c r="E214">
+        <v>0</v>
+      </c>
+      <c r="F214" t="s">
+        <v>396</v>
+      </c>
+      <c r="G214" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="215" spans="5:7">
+      <c r="E215">
+        <v>0</v>
+      </c>
+      <c r="F215" t="s">
+        <v>397</v>
+      </c>
+      <c r="G215" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="216" spans="5:7">
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216" t="s">
+        <v>398</v>
+      </c>
+      <c r="G216" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="217" spans="5:7">
+      <c r="E217">
+        <v>0</v>
+      </c>
+      <c r="F217" t="s">
+        <v>399</v>
+      </c>
+      <c r="G217" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="218" spans="5:7">
+      <c r="E218">
+        <v>0</v>
+      </c>
+      <c r="F218" t="s">
+        <v>400</v>
+      </c>
+      <c r="G218" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="219" spans="5:7">
+      <c r="E219">
+        <v>0</v>
+      </c>
+      <c r="F219" t="s">
+        <v>401</v>
+      </c>
+      <c r="G219" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="220" spans="5:7">
+      <c r="E220">
+        <v>0</v>
+      </c>
+      <c r="F220" t="s">
+        <v>402</v>
+      </c>
+      <c r="G220" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="221" spans="5:7">
+      <c r="E221">
+        <v>0</v>
+      </c>
+      <c r="F221" t="s">
+        <v>410</v>
+      </c>
+      <c r="G221" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="222" spans="5:7">
+      <c r="E222">
+        <v>0</v>
+      </c>
+      <c r="F222" t="s">
+        <v>403</v>
+      </c>
+      <c r="G222" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="223" spans="5:7">
+      <c r="E223">
+        <v>0</v>
+      </c>
+      <c r="F223" t="s">
+        <v>404</v>
+      </c>
+      <c r="G223" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="224" spans="5:7">
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224" t="s">
+        <v>405</v>
+      </c>
+      <c r="G224" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="225" spans="5:7">
+      <c r="E225">
+        <v>0</v>
+      </c>
+      <c r="F225" t="s">
+        <v>406</v>
+      </c>
+      <c r="G225" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="226" spans="5:7">
+      <c r="E226">
+        <v>0</v>
+      </c>
+      <c r="F226" t="s">
+        <v>407</v>
+      </c>
+      <c r="G226" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="227" spans="5:7">
+      <c r="E227">
+        <v>0</v>
+      </c>
+      <c r="F227" t="s">
+        <v>408</v>
+      </c>
+      <c r="G227" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="228" spans="5:7">
+      <c r="E228">
+        <v>0</v>
+      </c>
+      <c r="F228" t="s">
+        <v>409</v>
+      </c>
+      <c r="G228" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="229" spans="5:7">
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229" t="s">
+        <v>411</v>
+      </c>
+      <c r="G229" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="230" spans="5:7">
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230" t="s">
+        <v>412</v>
+      </c>
+      <c r="G230" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="231" spans="5:7">
+      <c r="E231">
+        <v>0</v>
+      </c>
+      <c r="F231" t="s">
+        <v>413</v>
+      </c>
+      <c r="G231" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="232" spans="5:7">
+      <c r="E232">
+        <v>0</v>
+      </c>
+      <c r="F232" t="s">
+        <v>414</v>
+      </c>
+      <c r="G232" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="233" spans="5:7">
+      <c r="E233">
+        <v>0</v>
+      </c>
+      <c r="F233" t="s">
+        <v>415</v>
+      </c>
+      <c r="G233" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="234" spans="5:7">
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="F234" t="s">
+        <v>416</v>
+      </c>
+      <c r="G234" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="235" spans="5:7">
+      <c r="E235">
+        <v>0</v>
+      </c>
+      <c r="F235" t="s">
+        <v>417</v>
+      </c>
+      <c r="G235" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: gitbook and pdf - index errors exist
</commit_message>
<xml_diff>
--- a/_index/index.xlsx
+++ b/_index/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pilha\pipetbooks\basic\_index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77CD5CF-3C79-4561-8589-210CAAB256A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A60528-1BFB-4566-8F44-795903E0BA00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECD2918D-62A0-4856-BE13-E9328C629C28}"/>
   </bookViews>
@@ -1662,8 +1662,8 @@
   <dimension ref="A1:I235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F155" sqref="F155"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L226" sqref="L226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>